<commit_message>
pushing up latest assemblies
</commit_message>
<xml_diff>
--- a/TestData/Transitor Batch - Copy.xlsx
+++ b/TestData/Transitor Batch - Copy.xlsx
@@ -23,6 +23,8 @@
     <sheet name="Raw data_outliers - (3)" sheetId="8" r:id="rId10"/>
     <sheet name="Raw data_discovery - (4)" sheetId="9" r:id="rId11"/>
     <sheet name="Raw data_outliers - (4)" sheetId="10" r:id="rId12"/>
+    <sheet name="Raw data_discovery - (5)" sheetId="11" r:id="rId13"/>
+    <sheet name="Raw data_outliers - (5)" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
@@ -2384,6 +2386,1174 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0">
+        <v>467</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0">
+        <v>467</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0">
+        <v>467</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>42</v>
+      </c>
+      <c r="B6" s="0">
+        <v>467</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>53</v>
+      </c>
+      <c r="B7" s="0">
+        <v>467</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0">
+        <v>502</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>62</v>
+      </c>
+      <c r="B10" s="0">
+        <v>502</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0">
+        <v>467</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>67</v>
+      </c>
+      <c r="B13" s="0">
+        <v>467</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>20</v>
+      </c>
+      <c r="B15" s="0">
+        <v>501</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>64</v>
+      </c>
+      <c r="B16" s="0">
+        <v>501</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>27</v>
+      </c>
+      <c r="B18" s="0">
+        <v>467</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>47</v>
+      </c>
+      <c r="B19" s="0">
+        <v>467</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>61</v>
+      </c>
+      <c r="B20" s="0">
+        <v>467</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0">
+        <v>503</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>65</v>
+      </c>
+      <c r="B23" s="0">
+        <v>503</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>34</v>
+      </c>
+      <c r="B25" s="0">
+        <v>467</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>56</v>
+      </c>
+      <c r="B26" s="0">
+        <v>467</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>37</v>
+      </c>
+      <c r="B28" s="0">
+        <v>501</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>48</v>
+      </c>
+      <c r="B29" s="0">
+        <v>501</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>38</v>
+      </c>
+      <c r="B31" s="0">
+        <v>478</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>82</v>
+      </c>
+      <c r="B32" s="0">
+        <v>478</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>41</v>
+      </c>
+      <c r="B34" s="0">
+        <v>498</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>86</v>
+      </c>
+      <c r="B35" s="0">
+        <v>498</v>
+      </c>
+      <c r="C35" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>50</v>
+      </c>
+      <c r="B37" s="0">
+        <v>467</v>
+      </c>
+      <c r="C37" s="0">
+        <v>0.766</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>84</v>
+      </c>
+      <c r="B38" s="0">
+        <v>467</v>
+      </c>
+      <c r="C38" s="0">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>63</v>
+      </c>
+      <c r="B40" s="0">
+        <v>478</v>
+      </c>
+      <c r="C40" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>71</v>
+      </c>
+      <c r="B41" s="0">
+        <v>478</v>
+      </c>
+      <c r="C41" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>76</v>
+      </c>
+      <c r="B43" s="0">
+        <v>457</v>
+      </c>
+      <c r="C43" s="0">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>77</v>
+      </c>
+      <c r="B44" s="0">
+        <v>457</v>
+      </c>
+      <c r="C44" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>81</v>
+      </c>
+      <c r="B46" s="0">
+        <v>459</v>
+      </c>
+      <c r="C46" s="0">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>88</v>
+      </c>
+      <c r="B47" s="0">
+        <v>459</v>
+      </c>
+      <c r="C47" s="0">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>95</v>
+      </c>
+      <c r="B49" s="0">
+        <v>501</v>
+      </c>
+      <c r="C49" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>98</v>
+      </c>
+      <c r="B50" s="0">
+        <v>501</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>100</v>
+      </c>
+      <c r="B51" s="0">
+        <v>501</v>
+      </c>
+      <c r="C51" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>453</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0">
+        <v>518</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.766</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0">
+        <v>464</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>477</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0">
+        <v>488</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0">
+        <v>503</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0">
+        <v>456</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0">
+        <v>458</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0">
+        <v>497</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0">
+        <v>490</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>14</v>
+      </c>
+      <c r="B12" s="0">
+        <v>472</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0">
+        <v>493</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0">
+        <v>494</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0">
+        <v>457</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0">
+        <v>473</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>25</v>
+      </c>
+      <c r="B17" s="0">
+        <v>486</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0">
+        <v>496</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>29</v>
+      </c>
+      <c r="B19" s="0">
+        <v>501</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>30</v>
+      </c>
+      <c r="B20" s="0">
+        <v>504</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>31</v>
+      </c>
+      <c r="B21" s="0">
+        <v>506</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>32</v>
+      </c>
+      <c r="B22" s="0">
+        <v>457</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>33</v>
+      </c>
+      <c r="B23" s="0">
+        <v>496</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>36</v>
+      </c>
+      <c r="B24" s="0">
+        <v>505</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>39</v>
+      </c>
+      <c r="B25" s="0">
+        <v>476</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>40</v>
+      </c>
+      <c r="B26" s="0">
+        <v>477</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>43</v>
+      </c>
+      <c r="B27" s="0">
+        <v>467</v>
+      </c>
+      <c r="C27" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>44</v>
+      </c>
+      <c r="B28" s="0">
+        <v>463</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>45</v>
+      </c>
+      <c r="B29" s="0">
+        <v>465</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>49</v>
+      </c>
+      <c r="B30" s="0">
+        <v>468</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>51</v>
+      </c>
+      <c r="B31" s="0">
+        <v>498</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>52</v>
+      </c>
+      <c r="B32" s="0">
+        <v>475</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>54</v>
+      </c>
+      <c r="B33" s="0">
+        <v>477</v>
+      </c>
+      <c r="C33" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>55</v>
+      </c>
+      <c r="B34" s="0">
+        <v>506</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>57</v>
+      </c>
+      <c r="B35" s="0">
+        <v>488</v>
+      </c>
+      <c r="C35" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>58</v>
+      </c>
+      <c r="B36" s="0">
+        <v>491</v>
+      </c>
+      <c r="C36" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>59</v>
+      </c>
+      <c r="B37" s="0">
+        <v>490</v>
+      </c>
+      <c r="C37" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>60</v>
+      </c>
+      <c r="B38" s="0">
+        <v>501</v>
+      </c>
+      <c r="C38" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>66</v>
+      </c>
+      <c r="B39" s="0">
+        <v>463</v>
+      </c>
+      <c r="C39" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>68</v>
+      </c>
+      <c r="B40" s="0">
+        <v>467</v>
+      </c>
+      <c r="C40" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>69</v>
+      </c>
+      <c r="B41" s="0">
+        <v>455</v>
+      </c>
+      <c r="C41" s="0">
+        <v>0.763</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>70</v>
+      </c>
+      <c r="B42" s="0">
+        <v>458</v>
+      </c>
+      <c r="C42" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>72</v>
+      </c>
+      <c r="B43" s="0">
+        <v>479</v>
+      </c>
+      <c r="C43" s="0">
+        <v>0.766</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>73</v>
+      </c>
+      <c r="B44" s="0">
+        <v>506</v>
+      </c>
+      <c r="C44" s="0">
+        <v>0.759</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>74</v>
+      </c>
+      <c r="B45" s="0">
+        <v>459</v>
+      </c>
+      <c r="C45" s="0">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>75</v>
+      </c>
+      <c r="B46" s="0">
+        <v>452</v>
+      </c>
+      <c r="C46" s="0">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>78</v>
+      </c>
+      <c r="B47" s="0">
+        <v>463</v>
+      </c>
+      <c r="C47" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>79</v>
+      </c>
+      <c r="B48" s="0">
+        <v>467</v>
+      </c>
+      <c r="C48" s="0">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>80</v>
+      </c>
+      <c r="B49" s="0">
+        <v>454</v>
+      </c>
+      <c r="C49" s="0">
+        <v>0.763</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>83</v>
+      </c>
+      <c r="B50" s="0">
+        <v>468</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0.763</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>85</v>
+      </c>
+      <c r="B51" s="0">
+        <v>487</v>
+      </c>
+      <c r="C51" s="0">
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>87</v>
+      </c>
+      <c r="B52" s="0">
+        <v>456</v>
+      </c>
+      <c r="C52" s="0">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>89</v>
+      </c>
+      <c r="B53" s="0">
+        <v>497</v>
+      </c>
+      <c r="C53" s="0">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>90</v>
+      </c>
+      <c r="B54" s="0">
+        <v>482</v>
+      </c>
+      <c r="C54" s="0">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>91</v>
+      </c>
+      <c r="B55" s="0">
+        <v>487</v>
+      </c>
+      <c r="C55" s="0">
+        <v>0.768</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>92</v>
+      </c>
+      <c r="B56" s="0">
+        <v>490</v>
+      </c>
+      <c r="C56" s="0">
+        <v>0.756</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>93</v>
+      </c>
+      <c r="B57" s="0">
+        <v>487</v>
+      </c>
+      <c r="C57" s="0">
+        <v>0.789</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>94</v>
+      </c>
+      <c r="B58" s="0">
+        <v>469</v>
+      </c>
+      <c r="C58" s="0">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>96</v>
+      </c>
+      <c r="B59" s="0">
+        <v>461</v>
+      </c>
+      <c r="C59" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>97</v>
+      </c>
+      <c r="B60" s="0">
+        <v>464</v>
+      </c>
+      <c r="C60" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>99</v>
+      </c>
+      <c r="B61" s="0">
+        <v>465</v>
+      </c>
+      <c r="C61" s="0">
+        <v>0.761</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D101"/>

</xml_diff>